<commit_message>
Women data pre-cleaned, all vizualizations updated for 11 events of men
</commit_message>
<xml_diff>
--- a/data/women/W_2019_12_Cup_USK.xlsx
+++ b/data/women/W_2019_12_Cup_USK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\data\women\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3992C213-C3AF-41E3-ACB7-5B60AFC07693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB1729E-EBFC-4CF4-BBCE-23B2A62DB4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11112" yWindow="-15588" windowWidth="15228" windowHeight="12360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1152" yWindow="-16176" windowWidth="18624" windowHeight="16392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initiation" sheetId="1" r:id="rId1"/>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1560,7 +1560,7 @@
   </sheetData>
   <autoFilter ref="A1:F43" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F43">
-      <sortCondition ref="A1"/>
+      <sortCondition ref="B1:B43"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1572,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA23FFA4-FC48-412F-A585-742B04BD9237}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1626,32 +1626,32 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H2">
-        <f>G2-I2</f>
-        <v>11</v>
+        <f t="shared" ref="H2:H43" si="0">G2-I2</f>
+        <v>20</v>
       </c>
       <c r="I2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>73</v>
@@ -1668,10 +1668,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1680,20 +1680,20 @@
         <v>64</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H43" si="0">G3-I3</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="I3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
         <v>73</v>
@@ -1710,32 +1710,32 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
       </c>
       <c r="E4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="I4">
-        <v>17</v>
+        <v>-19</v>
       </c>
       <c r="J4" t="s">
         <v>73</v>
@@ -1752,32 +1752,32 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
         <v>73</v>
@@ -1836,32 +1836,32 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0.83333333333333337</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G7">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I7">
-        <v>13</v>
+        <v>-4</v>
       </c>
       <c r="J7" t="s">
         <v>73</v>
@@ -1878,32 +1878,32 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I8">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s">
         <v>73</v>
@@ -1920,32 +1920,32 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>0.83333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="G9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>73</v>
@@ -1962,32 +1962,32 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G10">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I10">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="J10" t="s">
         <v>73</v>
@@ -2004,32 +2004,32 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G11">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J11" t="s">
         <v>73</v>
@@ -2046,32 +2046,32 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>64</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I12">
-        <v>9</v>
+        <v>-22</v>
       </c>
       <c r="J12" t="s">
         <v>73</v>
@@ -2088,10 +2088,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -2100,20 +2100,20 @@
         <v>64</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F13">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J13" t="s">
         <v>73</v>
@@ -2130,10 +2130,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -2142,20 +2142,20 @@
         <v>64</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I14">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
         <v>73</v>
@@ -2172,32 +2172,32 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
         <v>64</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G15">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J15" t="s">
         <v>73</v>
@@ -2214,32 +2214,32 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
       </c>
       <c r="E16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>-15</v>
       </c>
       <c r="J16" t="s">
         <v>73</v>
@@ -2256,32 +2256,32 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>64</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G17">
         <v>24</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
         <v>73</v>
@@ -2298,32 +2298,32 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G18">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>-9</v>
       </c>
       <c r="J18" t="s">
         <v>73</v>
@@ -2340,32 +2340,32 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>64</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19">
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G19">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I19">
-        <v>-1</v>
+        <v>-11</v>
       </c>
       <c r="J19" t="s">
         <v>73</v>
@@ -2382,32 +2382,32 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I20">
-        <v>6</v>
+        <v>-19</v>
       </c>
       <c r="J20" t="s">
         <v>73</v>
@@ -2424,32 +2424,32 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G21">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="I21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J21" t="s">
         <v>73</v>
@@ -2466,32 +2466,32 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>64</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G22">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="J22" t="s">
         <v>73</v>
@@ -2508,13 +2508,13 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
@@ -2526,14 +2526,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>-10</v>
       </c>
       <c r="J23" t="s">
         <v>73</v>
@@ -2550,13 +2550,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>64</v>
@@ -2568,14 +2568,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G24">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>-11</v>
       </c>
       <c r="J24" t="s">
         <v>73</v>
@@ -2592,13 +2592,13 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>64</v>
@@ -2610,14 +2610,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G25">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="J25" t="s">
         <v>73</v>
@@ -2634,10 +2634,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2646,20 +2646,20 @@
         <v>64</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="G26">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I26">
-        <v>-3</v>
+        <v>5</v>
       </c>
       <c r="J26" t="s">
         <v>73</v>
@@ -2676,32 +2676,32 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
         <v>64</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>0.33333333333333331</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G27">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I27">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="J27" t="s">
         <v>73</v>
@@ -2718,32 +2718,32 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>64</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F28">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I28">
-        <v>-5</v>
+        <v>17</v>
       </c>
       <c r="J28" t="s">
         <v>73</v>
@@ -2760,13 +2760,13 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>64</v>
@@ -2778,14 +2778,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G29">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I29">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="J29" t="s">
         <v>73</v>
@@ -2802,13 +2802,13 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>64</v>
@@ -2820,14 +2820,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G30">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="I30">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="J30" t="s">
         <v>73</v>
@@ -2844,13 +2844,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
         <v>64</v>
@@ -2862,14 +2862,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G31">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I31">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="J31" t="s">
         <v>73</v>
@@ -2886,32 +2886,32 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
         <v>64</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G32">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="I32">
-        <v>-9</v>
+        <v>8</v>
       </c>
       <c r="J32" t="s">
         <v>73</v>
@@ -2928,32 +2928,32 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I33">
-        <v>-10</v>
+        <v>19</v>
       </c>
       <c r="J33" t="s">
         <v>73</v>
@@ -2970,13 +2970,13 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
         <v>64</v>
@@ -2988,14 +2988,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G34">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I34">
-        <v>-11</v>
+        <v>-6</v>
       </c>
       <c r="J34" t="s">
         <v>73</v>
@@ -3012,13 +3012,13 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
@@ -3030,14 +3030,14 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="G35">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="I35">
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="J35" t="s">
         <v>73</v>
@@ -3054,32 +3054,32 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
         <v>64</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>0.33333333333333331</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G36">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="I36">
-        <v>-13</v>
+        <v>9</v>
       </c>
       <c r="J36" t="s">
         <v>73</v>
@@ -3096,29 +3096,29 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
         <v>64</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F37">
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G37">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H37">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I37">
         <v>-5</v>
@@ -3138,32 +3138,32 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
         <v>64</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>0.16666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G38">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="I38">
-        <v>-6</v>
+        <v>8</v>
       </c>
       <c r="J38" t="s">
         <v>73</v>
@@ -3222,32 +3222,32 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G40">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H40">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I40">
-        <v>-15</v>
+        <v>2</v>
       </c>
       <c r="J40" t="s">
         <v>73</v>
@@ -3264,32 +3264,32 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>64</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G41">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H41">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I41">
-        <v>-19</v>
+        <v>9</v>
       </c>
       <c r="J41" t="s">
         <v>73</v>
@@ -3306,32 +3306,32 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
         <v>64</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G42">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="H42">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I42">
-        <v>-19</v>
+        <v>13</v>
       </c>
       <c r="J42" t="s">
         <v>73</v>
@@ -3348,32 +3348,32 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="D43" t="s">
         <v>64</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G43">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H43">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I43">
-        <v>-22</v>
+        <v>-6</v>
       </c>
       <c r="J43" t="s">
         <v>73</v>
@@ -3389,7 +3389,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{DA23FFA4-FC48-412F-A585-742B04BD9237}"/>
+  <autoFilter ref="A1:M1" xr:uid="{DA23FFA4-FC48-412F-A585-742B04BD9237}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M43">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3399,8 +3403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA91E2E-F813-4D5B-8DDE-7F01E8593249}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3440,19 +3444,19 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="1">
-        <v>36325</v>
+        <v>37414</v>
       </c>
       <c r="F2" s="1">
         <v>43807</v>
@@ -3466,19 +3470,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="1">
-        <v>33018</v>
+        <v>37371</v>
       </c>
       <c r="F3" s="1">
         <v>43807</v>
@@ -3492,19 +3496,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="1">
-        <v>37371</v>
+        <v>26604</v>
       </c>
       <c r="F4" s="1">
         <v>43807</v>
@@ -3518,19 +3522,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
       </c>
       <c r="E5" s="1">
-        <v>33010</v>
+        <v>36617</v>
       </c>
       <c r="F5" s="1">
         <v>43807</v>
@@ -3544,19 +3548,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
       </c>
       <c r="E6" s="1">
-        <v>34911</v>
+        <v>37189</v>
       </c>
       <c r="F6" s="1">
         <v>43807</v>
@@ -3570,19 +3574,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="1">
-        <v>36429</v>
+        <v>32455</v>
       </c>
       <c r="F7" s="1">
         <v>43807</v>
@@ -3596,10 +3600,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -3608,7 +3612,7 @@
         <v>64</v>
       </c>
       <c r="E8" s="1">
-        <v>36130</v>
+        <v>33010</v>
       </c>
       <c r="F8" s="1">
         <v>43807</v>
@@ -3622,19 +3626,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
       </c>
       <c r="E9" s="1">
-        <v>36310</v>
+        <v>33437</v>
       </c>
       <c r="F9" s="1">
         <v>43807</v>
@@ -3648,19 +3652,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="1">
-        <v>37189</v>
+        <v>37509</v>
       </c>
       <c r="F10" s="1">
         <v>43807</v>
@@ -3674,19 +3678,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="1">
-        <v>37441</v>
+        <v>34902</v>
       </c>
       <c r="F11" s="1">
         <v>43807</v>
@@ -3700,19 +3704,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="1">
-        <v>36617</v>
+        <v>33956</v>
       </c>
       <c r="F12" s="1">
         <v>43807</v>
@@ -3726,19 +3730,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="1">
-        <v>36590</v>
+        <v>34628</v>
       </c>
       <c r="F13" s="1">
         <v>43807</v>
@@ -3752,19 +3756,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="1">
-        <v>36481</v>
+        <v>36590</v>
       </c>
       <c r="F14" s="1">
         <v>43807</v>
@@ -3778,19 +3782,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="1">
-        <v>36091</v>
+        <v>36590</v>
       </c>
       <c r="F15" s="1">
         <v>43807</v>
@@ -3804,19 +3808,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>64</v>
       </c>
       <c r="E16" s="1">
-        <v>33437</v>
+        <v>35863</v>
       </c>
       <c r="F16" s="1">
         <v>43807</v>
@@ -3830,19 +3834,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="1">
-        <v>36889</v>
+        <v>34873</v>
       </c>
       <c r="F17" s="1">
         <v>43807</v>
@@ -3856,19 +3860,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="1">
-        <v>34628</v>
+        <v>36889</v>
       </c>
       <c r="F18" s="1">
         <v>43807</v>
@@ -3882,19 +3886,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="1">
-        <v>37414</v>
+        <v>26851</v>
       </c>
       <c r="F19" s="1">
         <v>43807</v>
@@ -3908,19 +3912,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
       </c>
       <c r="E20" s="1">
-        <v>32792</v>
+        <v>35681</v>
       </c>
       <c r="F20" s="1">
         <v>43807</v>
@@ -3934,19 +3938,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
       </c>
       <c r="E21" s="1">
-        <v>34902</v>
+        <v>36091</v>
       </c>
       <c r="F21" s="1">
         <v>43807</v>
@@ -3960,19 +3964,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>64</v>
       </c>
       <c r="E22" s="1">
-        <v>36590</v>
+        <v>35259</v>
       </c>
       <c r="F22" s="1">
         <v>43807</v>
@@ -3986,19 +3990,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="1">
-        <v>36199</v>
+        <v>37200</v>
       </c>
       <c r="F23" s="1">
         <v>43807</v>
@@ -4012,19 +4016,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="1">
-        <v>34873</v>
+        <v>36404</v>
       </c>
       <c r="F24" s="1">
         <v>43807</v>
@@ -4038,19 +4042,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="1">
-        <v>37444</v>
+        <v>35577</v>
       </c>
       <c r="F25" s="1">
         <v>43807</v>
@@ -4064,10 +4068,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -4076,7 +4080,7 @@
         <v>64</v>
       </c>
       <c r="E26" s="1">
-        <v>37171</v>
+        <v>36130</v>
       </c>
       <c r="F26" s="1">
         <v>43807</v>
@@ -4090,19 +4094,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="1">
-        <v>37509</v>
+        <v>37401</v>
       </c>
       <c r="F27" s="1">
         <v>43807</v>
@@ -4116,19 +4120,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
         <v>64</v>
       </c>
       <c r="E28" s="1">
-        <v>32455</v>
+        <v>33018</v>
       </c>
       <c r="F28" s="1">
         <v>43807</v>
@@ -4142,19 +4146,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>64</v>
       </c>
       <c r="E29" s="1">
-        <v>35707</v>
+        <v>36310</v>
       </c>
       <c r="F29" s="1">
         <v>43807</v>
@@ -4168,19 +4172,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>64</v>
       </c>
       <c r="E30" s="1">
-        <v>35259</v>
+        <v>37444</v>
       </c>
       <c r="F30" s="1">
         <v>43807</v>
@@ -4194,19 +4198,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="1">
-        <v>37597</v>
+        <v>36199</v>
       </c>
       <c r="F31" s="1">
         <v>43807</v>
@@ -4220,19 +4224,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
         <v>64</v>
       </c>
       <c r="E32" s="1">
-        <v>36404</v>
+        <v>36481</v>
       </c>
       <c r="F32" s="1">
         <v>43807</v>
@@ -4246,19 +4250,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
       </c>
       <c r="E33" s="1">
-        <v>38143</v>
+        <v>36325</v>
       </c>
       <c r="F33" s="1">
         <v>43807</v>
@@ -4272,19 +4276,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
         <v>64</v>
       </c>
       <c r="E34" s="1">
-        <v>35577</v>
+        <v>37597</v>
       </c>
       <c r="F34" s="1">
         <v>43807</v>
@@ -4298,19 +4302,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" s="1">
-        <v>37200</v>
+        <v>36101</v>
       </c>
       <c r="F35" s="1">
         <v>43807</v>
@@ -4324,19 +4328,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="1">
-        <v>26851</v>
+        <v>34911</v>
       </c>
       <c r="F36" s="1">
         <v>43807</v>
@@ -4350,19 +4354,19 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="1">
-        <v>36101</v>
+        <v>35707</v>
       </c>
       <c r="F37" s="1">
         <v>43807</v>
@@ -4376,19 +4380,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="1">
-        <v>37401</v>
+        <v>36429</v>
       </c>
       <c r="F38" s="1">
         <v>43807</v>
@@ -4428,19 +4432,19 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
         <v>64</v>
       </c>
       <c r="E40" s="1">
-        <v>35863</v>
+        <v>32792</v>
       </c>
       <c r="F40" s="1">
         <v>43807</v>
@@ -4454,19 +4458,19 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>64</v>
       </c>
       <c r="E41" s="1">
-        <v>26604</v>
+        <v>37171</v>
       </c>
       <c r="F41" s="1">
         <v>43807</v>
@@ -4480,19 +4484,19 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
         <v>64</v>
       </c>
       <c r="E42" s="1">
-        <v>35681</v>
+        <v>37441</v>
       </c>
       <c r="F42" s="1">
         <v>43807</v>
@@ -4506,19 +4510,19 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="D43" t="s">
         <v>64</v>
       </c>
       <c r="E43" s="1">
-        <v>33956</v>
+        <v>38143</v>
       </c>
       <c r="F43" s="1">
         <v>43807</v>
@@ -4531,7 +4535,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{6CA91E2E-F813-4D5B-8DDE-7F01E8593249}"/>
+  <autoFilter ref="A1:H1" xr:uid="{6CA91E2E-F813-4D5B-8DDE-7F01E8593249}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13425,8 +13433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CFA784-5D81-4A15-A22C-1FCE7244A298}">
   <dimension ref="A1:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>